<commit_message>
Fixed the placeholder text not appearing  after clicking the entry field once
</commit_message>
<xml_diff>
--- a/Midterms.xlsx
+++ b/Midterms.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,34 +470,170 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>MAT 120 (Midterm 1)</t>
+          <t>CNG 242 (Quiz 1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>2023-11-19 Sunday 09:40</t>
+          <t>2024-03-29 Friday 16:40</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>S-122, S-123, S-124</t>
+          <t>I-103, I-104, I-105, I-106</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>MAT 120 (Midterm 2)</t>
+          <t>STAS 221 (Midterm 1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>2023-12-17 Sunday 09:40</t>
+          <t>2024-03-31 Sunday 15:40</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>S-122, S-123, S-124</t>
+          <t>S-119, S-121, S-122</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>TUR 102 (Midterm 1)</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-02 Tuesday 17:40</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>SZ-22, SZ-23, SZ-24, SZ-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>CNG 242 (Midterm 1)</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-16 Tuesday 17:40</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>SZ-22, SZ-23, SZ-24, SZ-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>CNG 232 (Midterm 1)</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-21 Sunday 14:40</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>S-121, S-122, S-123</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>CNG 280 (Midterm 1)</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-27 Saturday 13:40</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>I-103, I-104, I-105, I-106, IZ-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>CNG 242 (Quiz 2)</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-03 Friday 16:40</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>I-103, I-104, I-105, I-106</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>STAS 221 (Midterm 2)</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-12 Sunday 15:40</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>S-119, S-121, S-122</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>CNG 242 (Quiz 3)</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-17 Friday 16:40</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>I-103, I-104, I-105, I-106</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>CNG 242 (Quiz 4)</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-31 Friday 16:40</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>I-103, I-104, I-105, I-106</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added days until and days between to the final workbook
</commit_message>
<xml_diff>
--- a/Midterms.xlsx
+++ b/Midterms.xlsx
@@ -70,8 +70,12 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -437,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,8 +450,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="40" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="80" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="80" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,10 +464,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Days Until</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Days Between</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Classrooms</t>
         </is>
@@ -470,170 +486,400 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>CNG 242 (Quiz 1)</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>2024-03-29 Friday 16:40</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>I-103, I-104, I-105, I-106</t>
+          <t>CNG 140 (Quiz 1 - S1)</t>
+        </is>
+      </c>
+      <c r="B2" s="2">
+        <f>MAX(DATEVALUE(LEFT(D2, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C2" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D2, 10)) - DATEVALUE(LEFT(D1, 10)), B2)</f>
+        <v/>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>2024-03-15 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>I-103, I-104</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>STAS 221 (Midterm 1)</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>2024-03-31 Sunday 15:40</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>S-119, S-121, S-122</t>
+          <t>CNG 140 (Quiz 1 - S2)</t>
+        </is>
+      </c>
+      <c r="B3" s="2">
+        <f>MAX(DATEVALUE(LEFT(D3, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C3" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D3, 10)) - DATEVALUE(LEFT(D2, 10)), B3)</f>
+        <v/>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>2024-03-15 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>RZ-03</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>TUR 102 (Midterm 1)</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>2024-04-02 Tuesday 17:40</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>SZ-22, SZ-23, SZ-24, SZ-25</t>
+          <t>CNG 140 (Quiz 1 - S4)</t>
+        </is>
+      </c>
+      <c r="B4" s="2">
+        <f>MAX(DATEVALUE(LEFT(D4, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C4" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D4, 10)) - DATEVALUE(LEFT(D3, 10)), B4)</f>
+        <v/>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>2024-03-15 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>I-106</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CNG 242 (Midterm 1)</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>2024-04-16 Tuesday 17:40</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>SZ-22, SZ-23, SZ-24, SZ-25</t>
+          <t>CNG 140 (Quiz 1 - S3)</t>
+        </is>
+      </c>
+      <c r="B5" s="2">
+        <f>MAX(DATEVALUE(LEFT(D5, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C5" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D5, 10)) - DATEVALUE(LEFT(D4, 10)), B5)</f>
+        <v/>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>2024-03-15 Friday 14:40</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>I-103, IZ-03</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>CNG 232 (Midterm 1)</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>2024-04-21 Sunday 14:40</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>S-121, S-122, S-123</t>
+          <t>CNG 140 (Quiz 1 - S5)</t>
+        </is>
+      </c>
+      <c r="B6" s="2">
+        <f>MAX(DATEVALUE(LEFT(D6, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C6" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D6, 10)) - DATEVALUE(LEFT(D5, 10)), B6)</f>
+        <v/>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>2024-03-15 Friday 14:40</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>I-106</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CNG 280 (Midterm 1)</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>2024-04-27 Saturday 13:40</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>I-103, I-104, I-105, I-106, IZ-04</t>
+          <t>CNG 140 (Quiz 2 - S1)</t>
+        </is>
+      </c>
+      <c r="B7" s="2">
+        <f>MAX(DATEVALUE(LEFT(D7, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C7" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D7, 10)) - DATEVALUE(LEFT(D6, 10)), B7)</f>
+        <v/>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-05 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>I-103, IZ-04</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CNG 242 (Quiz 2)</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>2024-05-03 Friday 16:40</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>I-103, I-104, I-105, I-106</t>
+          <t>CNG 140 (Quiz 2 - S2)</t>
+        </is>
+      </c>
+      <c r="B8" s="2">
+        <f>MAX(DATEVALUE(LEFT(D8, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C8" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D8, 10)) - DATEVALUE(LEFT(D7, 10)), B8)</f>
+        <v/>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-05 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>I-106</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>STAS 221 (Midterm 2)</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>2024-05-12 Sunday 15:40</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>S-119, S-121, S-122</t>
+          <t>CNG 140 (Quiz 2 - S4)</t>
+        </is>
+      </c>
+      <c r="B9" s="2">
+        <f>MAX(DATEVALUE(LEFT(D9, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C9" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D9, 10)) - DATEVALUE(LEFT(D8, 10)), B9)</f>
+        <v/>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-05 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>RZ-03</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CNG 242 (Quiz 3)</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>2024-05-17 Friday 16:40</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>I-103, I-104, I-105, I-106</t>
+          <t>CNG 140 (Quiz 2 - S3)</t>
+        </is>
+      </c>
+      <c r="B10" s="2">
+        <f>MAX(DATEVALUE(LEFT(D10, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C10" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D10, 10)) - DATEVALUE(LEFT(D9, 10)), B10)</f>
+        <v/>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-05 Friday 14:40</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>I-106, IZ-04</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>CNG 242 (Quiz 4)</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>2024-05-31 Friday 16:40</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>I-103, I-104, I-105, I-106</t>
+          <t>CNG 140 (Quiz 2 - S5)</t>
+        </is>
+      </c>
+      <c r="B11" s="2">
+        <f>MAX(DATEVALUE(LEFT(D11, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C11" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D11, 10)) - DATEVALUE(LEFT(D10, 10)), B11)</f>
+        <v/>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-05 Friday 14:40</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>I-103</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>CNG 140 (Midterm 1)</t>
+        </is>
+      </c>
+      <c r="B12" s="2">
+        <f>MAX(DATEVALUE(LEFT(D12, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C12" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D12, 10)) - DATEVALUE(LEFT(D11, 10)), B12)</f>
+        <v/>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>2024-04-15 Monday 17:40</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>I-103, I-104, I-106, IZ-03, IZ-04, RZ-03, RZ-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>CNG 140 (Quiz 3 - S1)</t>
+        </is>
+      </c>
+      <c r="B13" s="2">
+        <f>MAX(DATEVALUE(LEFT(D13, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C13" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D13, 10)) - DATEVALUE(LEFT(D12, 10)), B13)</f>
+        <v/>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-03 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>I-103, IZ-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>CNG 140 (Quiz 3 - S2)</t>
+        </is>
+      </c>
+      <c r="B14" s="2">
+        <f>MAX(DATEVALUE(LEFT(D14, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C14" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D14, 10)) - DATEVALUE(LEFT(D13, 10)), B14)</f>
+        <v/>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-03 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>I-106</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>CNG 140 (Quiz 3 - S4)</t>
+        </is>
+      </c>
+      <c r="B15" s="2">
+        <f>MAX(DATEVALUE(LEFT(D15, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C15" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D15, 10)) - DATEVALUE(LEFT(D14, 10)), B15)</f>
+        <v/>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-03 Friday 11:40</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>RZ-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>CNG 140 (Quiz 3 - S3)</t>
+        </is>
+      </c>
+      <c r="B16" s="2">
+        <f>MAX(DATEVALUE(LEFT(D16, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C16" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D16, 10)) - DATEVALUE(LEFT(D15, 10)), B16)</f>
+        <v/>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-03 Friday 14:40</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>I-106, IZ-04</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>CNG 140 (Quiz 3 - S5)</t>
+        </is>
+      </c>
+      <c r="B17" s="2">
+        <f>MAX(DATEVALUE(LEFT(D17, 10)) - TODAY(), 0)</f>
+        <v/>
+      </c>
+      <c r="C17" s="2">
+        <f>IFERROR(DATEVALUE(LEFT(D17, 10)) - DATEVALUE(LEFT(D16, 10)), B17)</f>
+        <v/>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-03 Friday 14:40</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>I-103</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed up some of the styling to make it better
</commit_message>
<xml_diff>
--- a/Midterms.xlsx
+++ b/Midterms.xlsx
@@ -29,7 +29,7 @@
       <sz val="16"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -39,6 +39,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00afafaf"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00d0d0d0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -68,13 +78,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,11 +468,12 @@
     <col width="40" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
-    <col width="80" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="26" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Course Exam</t>
@@ -482,406 +499,427 @@
           <t>Classrooms</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Grades</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="26" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 1 - S1)</t>
         </is>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <f>MAX(DATEVALUE(LEFT(D2, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D2, 10)) - DATEVALUE(LEFT(D1, 10)), B2)</f>
         <v/>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>2024-03-15 Friday 11:40</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>I-103, I-104</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="F2" s="4" t="n"/>
+    </row>
+    <row r="3" ht="26" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 1 - S2)</t>
         </is>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <f>MAX(DATEVALUE(LEFT(D3, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D3, 10)) - DATEVALUE(LEFT(D2, 10)), B3)</f>
         <v/>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>2024-03-15 Friday 11:40</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>RZ-03</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="F3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="26" customHeight="1">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 1 - S4)</t>
         </is>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <f>MAX(DATEVALUE(LEFT(D4, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D4, 10)) - DATEVALUE(LEFT(D3, 10)), B4)</f>
         <v/>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>2024-03-15 Friday 11:40</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>I-106</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="F4" s="4" t="n"/>
+    </row>
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 1 - S3)</t>
         </is>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <f>MAX(DATEVALUE(LEFT(D5, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D5, 10)) - DATEVALUE(LEFT(D4, 10)), B5)</f>
         <v/>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>2024-03-15 Friday 14:40</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>I-103, IZ-03</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="F5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 1 - S5)</t>
         </is>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <f>MAX(DATEVALUE(LEFT(D6, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D6, 10)) - DATEVALUE(LEFT(D5, 10)), B6)</f>
         <v/>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>2024-03-15 Friday 14:40</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>I-106</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="F6" s="4" t="n"/>
+    </row>
+    <row r="7" ht="26" customHeight="1">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 2 - S1)</t>
         </is>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <f>MAX(DATEVALUE(LEFT(D7, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D7, 10)) - DATEVALUE(LEFT(D6, 10)), B7)</f>
         <v/>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>2024-04-05 Friday 11:40</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>I-103, IZ-04</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="F7" s="2" t="n"/>
+    </row>
+    <row r="8" ht="26" customHeight="1">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 2 - S2)</t>
         </is>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <f>MAX(DATEVALUE(LEFT(D8, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D8, 10)) - DATEVALUE(LEFT(D7, 10)), B8)</f>
         <v/>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>2024-04-05 Friday 11:40</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>I-106</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="F8" s="4" t="n"/>
+    </row>
+    <row r="9" ht="26" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 2 - S4)</t>
         </is>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <f>MAX(DATEVALUE(LEFT(D9, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D9, 10)) - DATEVALUE(LEFT(D8, 10)), B9)</f>
         <v/>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D9" s="1" t="inlineStr">
         <is>
           <t>2024-04-05 Friday 11:40</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="E9" s="1" t="inlineStr">
         <is>
           <t>RZ-03</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="F9" s="2" t="n"/>
+    </row>
+    <row r="10" ht="26" customHeight="1">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 2 - S3)</t>
         </is>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <f>MAX(DATEVALUE(LEFT(D10, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D10, 10)) - DATEVALUE(LEFT(D9, 10)), B10)</f>
         <v/>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>2024-04-05 Friday 14:40</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>I-106, IZ-04</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="F10" s="4" t="n"/>
+    </row>
+    <row r="11" ht="26" customHeight="1">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 2 - S5)</t>
         </is>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <f>MAX(DATEVALUE(LEFT(D11, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D11, 10)) - DATEVALUE(LEFT(D10, 10)), B11)</f>
         <v/>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="D11" s="1" t="inlineStr">
         <is>
           <t>2024-04-05 Friday 14:40</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr">
+      <c r="E11" s="1" t="inlineStr">
         <is>
           <t>I-103</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="F11" s="2" t="n"/>
+    </row>
+    <row r="12" ht="26" customHeight="1">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Midterm 1)</t>
         </is>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <f>MAX(DATEVALUE(LEFT(D12, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D12, 10)) - DATEVALUE(LEFT(D11, 10)), B12)</f>
         <v/>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>2024-04-15 Monday 17:40</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t>I-103, I-104, I-106, IZ-03, IZ-04, RZ-03, RZ-11</t>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="F12" s="4" t="n"/>
+    </row>
+    <row r="13" ht="26" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 3 - S1)</t>
         </is>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <f>MAX(DATEVALUE(LEFT(D13, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D13, 10)) - DATEVALUE(LEFT(D12, 10)), B13)</f>
         <v/>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="D13" s="1" t="inlineStr">
         <is>
           <t>2024-05-03 Friday 11:40</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="E13" s="1" t="inlineStr">
         <is>
           <t>I-103, IZ-04</t>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="F13" s="2" t="n"/>
+    </row>
+    <row r="14" ht="26" customHeight="1">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 3 - S2)</t>
         </is>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <f>MAX(DATEVALUE(LEFT(D14, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D14, 10)) - DATEVALUE(LEFT(D13, 10)), B14)</f>
         <v/>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="D14" s="3" t="inlineStr">
         <is>
           <t>2024-05-03 Friday 11:40</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
+      <c r="E14" s="3" t="inlineStr">
         <is>
           <t>I-106</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="F14" s="4" t="n"/>
+    </row>
+    <row r="15" ht="26" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 3 - S4)</t>
         </is>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <f>MAX(DATEVALUE(LEFT(D15, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D15, 10)) - DATEVALUE(LEFT(D14, 10)), B15)</f>
         <v/>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="D15" s="1" t="inlineStr">
         <is>
           <t>2024-05-03 Friday 11:40</t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="E15" s="1" t="inlineStr">
         <is>
           <t>RZ-03</t>
         </is>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="F15" s="2" t="n"/>
+    </row>
+    <row r="16" ht="26" customHeight="1">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 3 - S3)</t>
         </is>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <f>MAX(DATEVALUE(LEFT(D16, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <f>IFERROR(DATEVALUE(LEFT(D16, 10)) - DATEVALUE(LEFT(D15, 10)), B16)</f>
         <v/>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="D16" s="3" t="inlineStr">
         <is>
           <t>2024-05-03 Friday 14:40</t>
         </is>
       </c>
-      <c r="E16" s="2" t="inlineStr">
+      <c r="E16" s="3" t="inlineStr">
         <is>
           <t>I-106, IZ-04</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="F16" s="4" t="n"/>
+    </row>
+    <row r="17" ht="26" customHeight="1">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>CNG 140 (Quiz 3 - S5)</t>
         </is>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <f>MAX(DATEVALUE(LEFT(D17, 10)) - TODAY(), 0)</f>
         <v/>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <f>IFERROR(DATEVALUE(LEFT(D17, 10)) - DATEVALUE(LEFT(D16, 10)), B17)</f>
         <v/>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="D17" s="1" t="inlineStr">
         <is>
           <t>2024-05-03 Friday 14:40</t>
         </is>
       </c>
-      <c r="E17" s="2" t="inlineStr">
+      <c r="E17" s="1" t="inlineStr">
         <is>
           <t>I-103</t>
         </is>
       </c>
+      <c r="F17" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>